<commit_message>
Notes till 2 sample tests
</commit_message>
<xml_diff>
--- a/0DSAI_Estimation_notes.xlsx
+++ b/0DSAI_Estimation_notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aloksingh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aloksingh/Desktop/IIMB-DSAI-2025-26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D66D2D-9D78-234D-99C9-9060352E2C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F25282-7353-A344-909D-165D4CC353F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Camera Case" sheetId="18" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="145">
   <si>
     <t>Observation</t>
   </si>
@@ -815,6 +815,12 @@
   <si>
     <t xml:space="preserve">Chi is sum of squares </t>
   </si>
+  <si>
+    <t>Probablilty</t>
+  </si>
+  <si>
+    <t>MEAN +- ZSCOERE*SE</t>
+  </si>
 </sst>
 </file>
 
@@ -1131,7 +1137,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1375,6 +1381,9 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -8371,16 +8380,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>426</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>78761</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9392154</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>366</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>643211</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>142261</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>564443</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>157281</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8403,8 +8412,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15400510" y="6236660"/>
-          <a:ext cx="2286314" cy="2368710"/>
+          <a:off x="12339808" y="1709378"/>
+          <a:ext cx="4452413" cy="4484323"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11641,8 +11650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8212E896-07DB-4942-9E7E-1496D50F7DC6}">
   <dimension ref="A1:AX111"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="86" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView zoomScale="86" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13885,10 +13894,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CD7927-AEB3-A143-A32E-D41610D5B1A7}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13984,17 +13993,17 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -14002,25 +14011,41 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H22" s="89" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" s="99">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K22" s="97">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="53" t="s">
         <v>114</v>
       </c>
       <c r="B23" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="K23" s="98">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L23">
+        <f>0.5/100</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="53" t="s">
         <v>115</v>
       </c>
@@ -14028,7 +14053,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -14036,17 +14061,25 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <f>_xlfn.NORM.S.INV(0.005)</f>
+        <v>-2.5758293035488999</v>
+      </c>
+      <c r="J27">
+        <f>_xlfn.NORM.S.INV(0.995)</f>
+        <v>2.5758293035488999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -14054,7 +14087,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>110</v>
       </c>
@@ -14064,6 +14097,12 @@
       </c>
       <c r="D32" s="83" t="s">
         <v>99</v>
+      </c>
+      <c r="I32" s="98">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J32">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -25926,10 +25965,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AEF9CDD-FC8C-4A0A-A67F-A1C5996C85F4}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25937,7 +25976,7 @@
     <col min="1" max="1" width="8.83203125" style="7"/>
     <col min="2" max="2" width="11.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="7"/>
-    <col min="4" max="4" width="15.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" style="7" customWidth="1"/>
     <col min="6" max="6" width="4" style="7" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" style="7" customWidth="1"/>
@@ -26228,34 +26267,47 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="Q17" s="7">
         <f>_xlfn.NORM.S.INV(0.01)</f>
         <v>-2.3263478740408408</v>
       </c>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="88">
+        <f>_xlfn.NORM.S.INV(0.005)</f>
+        <v>-2.5758293035488999</v>
+      </c>
+      <c r="C20" s="7">
+        <f>_xlfn.NORM.S.INV(0.995)</f>
+        <v>2.5758293035488999</v>
+      </c>
       <c r="E20" s="88">
         <f>_xlfn.NORM.S.INV(0.975)</f>
         <v>1.9599639845400536</v>
       </c>
     </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E21" s="88">
         <f>_xlfn.NORM.S.INV(0.025)</f>
         <v>-1.9599639845400538</v>
       </c>
     </row>
-    <row r="23" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E23" s="88">
         <f>_xlfn.NORM.S.INV(0.95)</f>
         <v>1.6448536269514715</v>
       </c>
     </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E24" s="88">
         <f>_xlfn.NORM.S.INV(0.05)</f>
         <v>-1.6448536269514726</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D29" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -26270,10 +26322,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D7CE93-5F94-49A6-BFB6-3AB2DA4B0D0A}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26579,6 +26631,12 @@
       <c r="F23" s="7">
         <f>_xlfn.T.INV(0.025,35)</f>
         <v>-2.0301079282503438</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F29" s="88">
+        <f>_xlfn.T.INV(0.005,35)</f>
+        <v>-2.7238055892080912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>